<commit_message>
540 collection in blockes
</commit_message>
<xml_diff>
--- a/webscrapping school/msaces/Boletim_da_PI_-_2025-07-02.xlsx
+++ b/webscrapping school/msaces/Boletim_da_PI_-_2025-07-02.xlsx
@@ -539,11 +539,7 @@
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>(531) 27.5.22</t>
-        </is>
-      </c>
+      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -595,11 +591,7 @@
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>(531) 7.1.11 ; 14.5.2</t>
-        </is>
-      </c>
+      <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -651,11 +643,7 @@
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>(531) 25.5.94</t>
-        </is>
-      </c>
+      <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -679,11 +667,7 @@
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>(531) 27.5.4</t>
-        </is>
-      </c>
+      <c r="F9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -763,11 +747,7 @@
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>(531) 27.5.1</t>
-        </is>
-      </c>
+      <c r="F12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -791,11 +771,7 @@
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>(531) 7.3.2 ; 19.9.2 ; 26.11.9 ; 26.11.12</t>
-        </is>
-      </c>
+      <c r="F13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -847,11 +823,7 @@
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>(531) 27.5.1</t>
-        </is>
-      </c>
+      <c r="F15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -874,11 +846,7 @@
           <t>35</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>E INDUSTRIAL N.º 2025/07/02</t>
-        </is>
-      </c>
+      <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
     </row>
     <row r="17">
@@ -903,11 +871,7 @@
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>(531) 25.5.94</t>
-        </is>
-      </c>
+      <c r="F17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -987,11 +951,7 @@
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>(531) 27.5.1</t>
-        </is>
-      </c>
+      <c r="F20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1015,11 +975,7 @@
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>(531) 26.15.5</t>
-        </is>
-      </c>
+      <c r="F21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1099,11 +1055,7 @@
         </is>
       </c>
       <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>(531) 26.15.5</t>
-        </is>
-      </c>
+      <c r="F24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1240,7 +1192,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>ESCOLAS DE CONDUÇÃO</t>
+          <t>ESCOLAS DE CONDUÇÃO GRUPO LIDADOR DA MAIA</t>
         </is>
       </c>
       <c r="F29" t="inlineStr"/>
@@ -1266,11 +1218,7 @@
           <t>43</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>BOLETIM DA PROPRIEDADE</t>
-        </is>
-      </c>
+      <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr"/>
     </row>
     <row r="31">
@@ -1379,11 +1327,7 @@
         </is>
       </c>
       <c r="E34" t="inlineStr"/>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>(531) 1.13.2</t>
-        </is>
-      </c>
+      <c r="F34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1491,11 +1435,7 @@
         </is>
       </c>
       <c r="E38" t="inlineStr"/>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>(531) 24.17.25 ; 27.3.15 ; 27.5.1 ; 29.1.4</t>
-        </is>
-      </c>
+      <c r="F38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1518,11 +1458,7 @@
           <t>25</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>E INDUSTRIAL N.º 2025/07/02</t>
-        </is>
-      </c>
+      <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr"/>
     </row>
     <row r="40">
@@ -1574,11 +1510,7 @@
           <t>30</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>E INDUSTRIAL N.º 2025/07/02</t>
-        </is>
-      </c>
+      <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr"/>
     </row>
     <row r="42">
@@ -1631,11 +1563,7 @@
         </is>
       </c>
       <c r="E43" t="inlineStr"/>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>(531) 27.3.15 ; 27.5.1</t>
-        </is>
-      </c>
+      <c r="F43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1659,11 +1587,7 @@
         </is>
       </c>
       <c r="E44" t="inlineStr"/>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>(531) 1.15.21 ; 5.3.14 ; 19.1.4 ; 27.3.15 ; 27.5.10 ; 29.1.99</t>
-        </is>
-      </c>
+      <c r="F44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1715,11 +1639,7 @@
         </is>
       </c>
       <c r="E46" t="inlineStr"/>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>(531) 26.1.18</t>
-        </is>
-      </c>
+      <c r="F46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1743,11 +1663,7 @@
         </is>
       </c>
       <c r="E47" t="inlineStr"/>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>(531) 18.5.3 ; 26.11.13</t>
-        </is>
-      </c>
+      <c r="F47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1771,11 +1687,7 @@
         </is>
       </c>
       <c r="E48" t="inlineStr"/>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>(531) 27.5.9 ; 27.5.10 ; 27.5.11 ; 27.5.13</t>
-        </is>
-      </c>
+      <c r="F48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1798,11 +1710,7 @@
           <t>16</t>
         </is>
       </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>BOLETIM DA PROPRIEDADE</t>
-        </is>
-      </c>
+      <c r="E49" t="inlineStr"/>
       <c r="F49" t="inlineStr"/>
     </row>
     <row r="50">
@@ -1911,11 +1819,7 @@
         </is>
       </c>
       <c r="E53" t="inlineStr"/>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>(531) 26.1.3 ; 26.1.18 ; 27.99.1 ; 29.1.3 ; 29.1.98</t>
-        </is>
-      </c>
+      <c r="F53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1995,11 +1899,7 @@
         </is>
       </c>
       <c r="E56" t="inlineStr"/>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>(531) 27.5.10</t>
-        </is>
-      </c>
+      <c r="F56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2023,11 +1923,7 @@
         </is>
       </c>
       <c r="E57" t="inlineStr"/>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>(531) 26.3.1 ; 26.11.7 ; 26.11.8</t>
-        </is>
-      </c>
+      <c r="F57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2051,11 +1947,7 @@
         </is>
       </c>
       <c r="E58" t="inlineStr"/>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>(531) 13.1.6</t>
-        </is>
-      </c>
+      <c r="F58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2079,11 +1971,7 @@
         </is>
       </c>
       <c r="E59" t="inlineStr"/>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>(531) 7.1.24</t>
-        </is>
-      </c>
+      <c r="F59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2135,11 +2023,7 @@
         </is>
       </c>
       <c r="E61" t="inlineStr"/>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t>(531) 26.1.6 ; 26.2.7 ; 26.3.4 ; 26.4.9 ; 29.1.13</t>
-        </is>
-      </c>
+      <c r="F61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2163,11 +2047,7 @@
         </is>
       </c>
       <c r="E62" t="inlineStr"/>
-      <c r="F62" t="inlineStr">
-        <is>
-          <t>(531) 27.5.17 ; 29.1.7 ; 29.1.97</t>
-        </is>
-      </c>
+      <c r="F62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2191,11 +2071,7 @@
         </is>
       </c>
       <c r="E63" t="inlineStr"/>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t>(531) 25.1.25</t>
-        </is>
-      </c>
+      <c r="F63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2220,7 +2096,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>SAVOR THE MIND'S</t>
+          <t>SAVOR THE MIND'S REBELLION</t>
         </is>
       </c>
       <c r="F64" t="inlineStr"/>
@@ -2322,11 +2198,7 @@
         </is>
       </c>
       <c r="D68" t="inlineStr"/>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>E INDUSTRIAL N.º 2025/07/02</t>
-        </is>
-      </c>
+      <c r="E68" t="inlineStr"/>
       <c r="F68" t="inlineStr"/>
     </row>
     <row r="69">
@@ -2347,11 +2219,7 @@
       </c>
       <c r="D69" t="inlineStr"/>
       <c r="E69" t="inlineStr"/>
-      <c r="F69" t="inlineStr">
-        <is>
-          <t>(531) 27.3.15 ; 27.5.1</t>
-        </is>
-      </c>
+      <c r="F69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">

</xml_diff>